<commit_message>
Update EAS package to E16
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASDTYPE/MS-ASDTYPE_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASDTYPE/MS-ASDTYPE_RequirementSpecification.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$141</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$144</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="300">
   <si>
     <t>Req ID</t>
   </si>
@@ -731,31 +731,7 @@
     <t>2.3.2</t>
   </si>
   <si>
-    <t>2.4</t>
-  </si>
-  <si>
     <t>2.5</t>
-  </si>
-  <si>
-    <t>2.6</t>
-  </si>
-  <si>
-    <t>2.6.1</t>
-  </si>
-  <si>
-    <t>2.6.2</t>
-  </si>
-  <si>
-    <t>2.6.3</t>
-  </si>
-  <si>
-    <t>2.6.4</t>
-  </si>
-  <si>
-    <t>2.6.5</t>
-  </si>
-  <si>
-    <t>2.7</t>
   </si>
   <si>
     <t>5</t>
@@ -1001,13 +977,7 @@
     <t>[In enumeration Data Type] In accordance with [XMLSCHEMA2/2] section 4.3.5, it is specified using the restriction element to declare the enumeration, and the enumeration element to define one or more allowed values.</t>
   </si>
   <si>
-    <t>[In integer Data Type] An integer is a numeric value that can be provided in the XML body of a command.</t>
-  </si>
-  <si>
     <t>[In integer Data Type] It [an integer] is an XML schema primitive data type, as specified in [XMLSCHEMA2/2] section 3.3.13.</t>
-  </si>
-  <si>
-    <t>[In integer Data Type] Elements with an integer data type MUST be encoded and transmitted as [WBXML1.2] inline strings.</t>
   </si>
   <si>
     <t>[In string Data Type] A string is a chunk of Unicode text.</t>
@@ -1123,66 +1093,103 @@
     <t>[In Compact DateTime] The format of a Compact DateTime value is specified by the following Augmented Backus-Naur Form (ABNF) notation.</t>
   </si>
   <si>
+    <t>[In unsignedByte Data Type] The unsignedByte data type is an integer value between 0 and 255, inclusive.</t>
+  </si>
+  <si>
+    <t>[In unsignedByte Data Type] It [unsignedByte]is an XML schema primitive data type as specified in [XMLSCHEMA2/2] section 3.3.24.</t>
+  </si>
+  <si>
+    <t>[In unsignedByte Data Type] Elements of this type [unsignedByte type] are declared with an element whose type attribute is set to "unsignedByte".</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
+  </si>
+  <si>
+    <t>Exchange ActiveSync: Data Types</t>
+  </si>
+  <si>
+    <t>[In Time Zones and Daylight Saving Time] [All times can be in device-local time, and]There is no need for time zones or Daylight Saving Time (DST).</t>
+  </si>
+  <si>
+    <t>[In Calculating Dates and Times] The stored UTC corresponds to the first occurrence of the series[, but later meetings can have different corresponding UTC times].</t>
+  </si>
+  <si>
+    <t>Open Specification Date:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-ASDTYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In double Data Type] A double is a floating point value. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In double Data Type] It is an XML schema primitive data type, as specified in [XMLSCHEMA2/2] section 3.2.5. </t>
+  </si>
+  <si>
+    <t>[In integer Data Type] An integer is a whole-number value.</t>
+  </si>
+  <si>
+    <t>2.7.1</t>
+  </si>
+  <si>
+    <t>2.7.2</t>
+  </si>
+  <si>
+    <t>2.7.3</t>
+  </si>
+  <si>
+    <t>2.7.4</t>
+  </si>
+  <si>
+    <t>2.7.5</t>
+  </si>
+  <si>
+    <t>MS-ASDTYPE_R500</t>
+  </si>
+  <si>
+    <t>MS-ASDTYPE_R501</t>
+  </si>
+  <si>
+    <t>MS-ASDTYPE_R502</t>
+  </si>
+  <si>
     <t>[In Compact DateTime] [The format of a Compact DateTime value is specified by the following Augmented Backus-Naur Form (ABNF) notation. ]
-date_string   = year month day "T" hour minute seconds [milliseconds] "Z"
+date_string   = year month day "T" hour minute seconds "Z"
 year          = 4*DIGIT
 month         = ("0" DIGIT) / "10" / "11" / "12"
 day           = ("0" DIGIT) / ("1" DIGIT) / ("2" DIGIT) / "30" / "31"
 hour          = ("0" DIGIT) / ("1" DIGIT) / "20" / "21" / "22" / "23"
 minute        = ("0" DIGIT) / ("1" DIGIT) / ("2" DIGIT) / ("3" DIGIT) / ("4" DIGIT) / ("5" DIGIT)
-seconds       = ("0" DIGIT) / ("1" DIGIT) / ("2" DIGIT) / ("3" DIGIT) / ("4" DIGIT) / ("5" DIGIT)
-milliseconds  = 1*3DIGIT</t>
-  </si>
-  <si>
-    <t>[In unsignedByte Data Type] The unsignedByte data type is an integer value between 0 and 255, inclusive.</t>
-  </si>
-  <si>
-    <t>[In unsignedByte Data Type] It [unsignedByte]is an XML schema primitive data type as specified in [XMLSCHEMA2/2] section 3.3.24.</t>
-  </si>
-  <si>
-    <t>[In unsignedByte Data Type] Elements of this type [unsignedByte type] are declared with an element whose type attribute is set to "unsignedByte".</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
-  </si>
-  <si>
-    <t>Exchange ActiveSync: Data Types</t>
-  </si>
-  <si>
-    <t>[In Time Zones and Daylight Saving Time] [All times can be in device-local time, and]There is no need for time zones or Daylight Saving Time (DST).</t>
-  </si>
-  <si>
-    <t>[In Calculating Dates and Times] The stored UTC corresponds to the first occurrence of the series[, but later meetings can have different corresponding UTC times].</t>
-  </si>
-  <si>
-    <t>12.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open Specification Date:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS-ASDTYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+seconds       = ("0" DIGIT) / ("1" DIGIT) / ("2" DIGIT) / ("3" DIGIT) / ("4" DIGIT) / ("5" DIGIT)</t>
+  </si>
+  <si>
+    <t>[In integer Data Type] Elements with an integer data type MUST be encoded and transmitted as WBXML inline strings, as specified in [WBXML1.2].</t>
+  </si>
+  <si>
+    <t>[In double Data Type] Elements with a double data type MUST be encoded and transmitted as WBXML inline strings, as specified in [WBXML1.2].</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1370,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1379,13 +1386,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1418,7 +1425,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1439,6 +1446,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1481,7 +1491,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
     <dxf>
@@ -2025,8 +2035,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I141" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I144" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I144"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -2073,7 +2083,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2360,28 +2370,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -2389,9 +2399,9 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2400,146 +2410,146 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="F3" s="12">
-        <v>41474</v>
+        <v>42185</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:10" ht="21">
+      <c r="A4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -2549,15 +2559,15 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -2567,15 +2577,15 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -2585,15 +2595,15 @@
       <c r="C14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -2603,64 +2613,64 @@
       <c r="C15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2690,7 +2700,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="23" customFormat="1">
       <c r="A20" s="22" t="s">
         <v>34</v>
       </c>
@@ -2698,7 +2708,7 @@
         <v>156</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -2709,7 +2719,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A21" s="22" t="s">
         <v>35</v>
       </c>
@@ -2717,7 +2727,7 @@
         <v>156</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -2728,7 +2738,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A22" s="22" t="s">
         <v>36</v>
       </c>
@@ -2736,7 +2746,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -2747,7 +2757,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A23" s="22" t="s">
         <v>37</v>
       </c>
@@ -2755,7 +2765,7 @@
         <v>157</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -2766,7 +2776,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A24" s="22" t="s">
         <v>38</v>
       </c>
@@ -2774,7 +2784,7 @@
         <v>157</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -2785,7 +2795,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A25" s="22" t="s">
         <v>39</v>
       </c>
@@ -2793,7 +2803,7 @@
         <v>157</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -2804,7 +2814,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A26" s="22" t="s">
         <v>40</v>
       </c>
@@ -2812,7 +2822,7 @@
         <v>157</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -2823,7 +2833,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A27" s="22" t="s">
         <v>41</v>
       </c>
@@ -2831,7 +2841,7 @@
         <v>158</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -2842,7 +2852,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A28" s="22" t="s">
         <v>42</v>
       </c>
@@ -2850,7 +2860,7 @@
         <v>158</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -2861,7 +2871,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A29" s="22" t="s">
         <v>43</v>
       </c>
@@ -2869,7 +2879,7 @@
         <v>158</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -2880,7 +2890,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A30" s="22" t="s">
         <v>44</v>
       </c>
@@ -2888,7 +2898,7 @@
         <v>159</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -2899,7 +2909,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A31" s="22" t="s">
         <v>45</v>
       </c>
@@ -2907,7 +2917,7 @@
         <v>159</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -2918,7 +2928,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="23" customFormat="1">
       <c r="A32" s="22" t="s">
         <v>46</v>
       </c>
@@ -2926,7 +2936,7 @@
         <v>159</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -2937,7 +2947,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="150" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="150">
       <c r="A33" s="22" t="s">
         <v>47</v>
       </c>
@@ -2945,7 +2955,7 @@
         <v>159</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -2956,7 +2966,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30">
       <c r="A34" s="29" t="s">
         <v>48</v>
       </c>
@@ -2964,7 +2974,7 @@
         <v>159</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
@@ -2975,7 +2985,7 @@
       <c r="H34" s="29"/>
       <c r="I34" s="31"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30">
       <c r="A35" s="29" t="s">
         <v>49</v>
       </c>
@@ -2983,7 +2993,7 @@
         <v>159</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
@@ -2994,7 +3004,7 @@
       <c r="H35" s="29"/>
       <c r="I35" s="31"/>
     </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="29" t="s">
         <v>50</v>
       </c>
@@ -3002,7 +3012,7 @@
         <v>159</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
@@ -3013,7 +3023,7 @@
       <c r="H36" s="29"/>
       <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="29" t="s">
         <v>51</v>
       </c>
@@ -3021,7 +3031,7 @@
         <v>159</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
@@ -3032,7 +3042,7 @@
       <c r="H37" s="29"/>
       <c r="I37" s="31"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="29" t="s">
         <v>52</v>
       </c>
@@ -3040,7 +3050,7 @@
         <v>160</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
@@ -3051,7 +3061,7 @@
       <c r="H38" s="29"/>
       <c r="I38" s="31"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="29" t="s">
         <v>53</v>
       </c>
@@ -3059,7 +3069,7 @@
         <v>160</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
@@ -3070,7 +3080,7 @@
       <c r="H39" s="29"/>
       <c r="I39" s="31"/>
     </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30">
       <c r="A40" s="29" t="s">
         <v>54</v>
       </c>
@@ -3078,7 +3088,7 @@
         <v>160</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
@@ -3089,7 +3099,7 @@
       <c r="H40" s="29"/>
       <c r="I40" s="31"/>
     </row>
-    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="45">
       <c r="A41" s="29" t="s">
         <v>55</v>
       </c>
@@ -3097,7 +3107,7 @@
         <v>160</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
@@ -3108,7 +3118,7 @@
       <c r="H41" s="29"/>
       <c r="I41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30">
       <c r="A42" s="29" t="s">
         <v>56</v>
       </c>
@@ -3116,7 +3126,7 @@
         <v>160</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
@@ -3127,7 +3137,7 @@
       <c r="H42" s="29"/>
       <c r="I42" s="31"/>
     </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30">
       <c r="A43" s="29" t="s">
         <v>57</v>
       </c>
@@ -3135,7 +3145,7 @@
         <v>160</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
@@ -3146,7 +3156,7 @@
       <c r="H43" s="29"/>
       <c r="I43" s="31"/>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="45">
       <c r="A44" s="29" t="s">
         <v>58</v>
       </c>
@@ -3154,7 +3164,7 @@
         <v>160</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
@@ -3165,7 +3175,7 @@
       <c r="H44" s="29"/>
       <c r="I44" s="31"/>
     </row>
-    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="60">
       <c r="A45" s="29" t="s">
         <v>59</v>
       </c>
@@ -3173,7 +3183,7 @@
         <v>160</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -3184,7 +3194,7 @@
       <c r="H45" s="29"/>
       <c r="I45" s="31"/>
     </row>
-    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="60">
       <c r="A46" s="29" t="s">
         <v>60</v>
       </c>
@@ -3192,7 +3202,7 @@
         <v>160</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29"/>
@@ -3203,7 +3213,7 @@
       <c r="H46" s="29"/>
       <c r="I46" s="31"/>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30">
       <c r="A47" s="29" t="s">
         <v>61</v>
       </c>
@@ -3211,7 +3221,7 @@
         <v>160</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
@@ -3222,7 +3232,7 @@
       <c r="H47" s="29"/>
       <c r="I47" s="31"/>
     </row>
-    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="60">
       <c r="A48" s="29" t="s">
         <v>62</v>
       </c>
@@ -3230,7 +3240,7 @@
         <v>160</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29"/>
@@ -3241,7 +3251,7 @@
       <c r="H48" s="29"/>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="60">
       <c r="A49" s="29" t="s">
         <v>63</v>
       </c>
@@ -3249,7 +3259,7 @@
         <v>160</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29"/>
@@ -3260,7 +3270,7 @@
       <c r="H49" s="29"/>
       <c r="I49" s="31"/>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30">
       <c r="A50" s="29" t="s">
         <v>64</v>
       </c>
@@ -3268,7 +3278,7 @@
         <v>160</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29"/>
@@ -3279,7 +3289,7 @@
       <c r="H50" s="29"/>
       <c r="I50" s="31"/>
     </row>
-    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="60">
       <c r="A51" s="29" t="s">
         <v>65</v>
       </c>
@@ -3287,7 +3297,7 @@
         <v>160</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29"/>
@@ -3298,7 +3308,7 @@
       <c r="H51" s="29"/>
       <c r="I51" s="31"/>
     </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="60">
       <c r="A52" s="29" t="s">
         <v>66</v>
       </c>
@@ -3306,7 +3316,7 @@
         <v>160</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
@@ -3317,7 +3327,7 @@
       <c r="H52" s="29"/>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30">
       <c r="A53" s="29" t="s">
         <v>67</v>
       </c>
@@ -3325,7 +3335,7 @@
         <v>160</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
@@ -3336,7 +3346,7 @@
       <c r="H53" s="29"/>
       <c r="I53" s="31"/>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="29" t="s">
         <v>68</v>
       </c>
@@ -3344,7 +3354,7 @@
         <v>160</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29"/>
@@ -3355,7 +3365,7 @@
       <c r="H54" s="29"/>
       <c r="I54" s="31"/>
     </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="45">
       <c r="A55" s="29" t="s">
         <v>69</v>
       </c>
@@ -3363,7 +3373,7 @@
         <v>160</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
@@ -3374,7 +3384,7 @@
       <c r="H55" s="29"/>
       <c r="I55" s="31"/>
     </row>
-    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="45">
       <c r="A56" s="29" t="s">
         <v>70</v>
       </c>
@@ -3382,7 +3392,7 @@
         <v>160</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29"/>
@@ -3393,7 +3403,7 @@
       <c r="H56" s="29"/>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="45">
       <c r="A57" s="29" t="s">
         <v>71</v>
       </c>
@@ -3401,7 +3411,7 @@
         <v>160</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="29"/>
@@ -3412,7 +3422,7 @@
       <c r="H57" s="29"/>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30">
       <c r="A58" s="29" t="s">
         <v>72</v>
       </c>
@@ -3420,7 +3430,7 @@
         <v>160</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29"/>
@@ -3431,7 +3441,7 @@
       <c r="H58" s="29"/>
       <c r="I58" s="31"/>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="45">
       <c r="A59" s="29" t="s">
         <v>73</v>
       </c>
@@ -3439,7 +3449,7 @@
         <v>160</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3450,7 +3460,7 @@
       <c r="H59" s="29"/>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="45">
       <c r="A60" s="29" t="s">
         <v>74</v>
       </c>
@@ -3458,7 +3468,7 @@
         <v>160</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="29"/>
@@ -3469,7 +3479,7 @@
       <c r="H60" s="29"/>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30">
       <c r="A61" s="29" t="s">
         <v>75</v>
       </c>
@@ -3477,7 +3487,7 @@
         <v>160</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
@@ -3488,7 +3498,7 @@
       <c r="H61" s="29"/>
       <c r="I61" s="31"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30">
       <c r="A62" s="29" t="s">
         <v>76</v>
       </c>
@@ -3496,7 +3506,7 @@
         <v>160</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29"/>
@@ -3507,7 +3517,7 @@
       <c r="H62" s="29"/>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="45">
       <c r="A63" s="29" t="s">
         <v>77</v>
       </c>
@@ -3515,7 +3525,7 @@
         <v>160</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29"/>
@@ -3526,7 +3536,7 @@
       <c r="H63" s="29"/>
       <c r="I63" s="31"/>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="45">
       <c r="A64" s="29" t="s">
         <v>78</v>
       </c>
@@ -3534,7 +3544,7 @@
         <v>160</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29"/>
@@ -3545,7 +3555,7 @@
       <c r="H64" s="29"/>
       <c r="I64" s="31"/>
     </row>
-    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="29" t="s">
         <v>79</v>
       </c>
@@ -3553,7 +3563,7 @@
         <v>160</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29"/>
@@ -3564,7 +3574,7 @@
       <c r="H65" s="29"/>
       <c r="I65" s="31"/>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="29" t="s">
         <v>80</v>
       </c>
@@ -3572,7 +3582,7 @@
         <v>160</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29"/>
@@ -3583,7 +3593,7 @@
       <c r="H66" s="29"/>
       <c r="I66" s="31"/>
     </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="30">
       <c r="A67" s="29" t="s">
         <v>81</v>
       </c>
@@ -3591,7 +3601,7 @@
         <v>160</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3602,7 +3612,7 @@
       <c r="H67" s="29"/>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="29" t="s">
         <v>82</v>
       </c>
@@ -3610,7 +3620,7 @@
         <v>161</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29"/>
@@ -3621,7 +3631,7 @@
       <c r="H68" s="29"/>
       <c r="I68" s="31"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="30">
       <c r="A69" s="29" t="s">
         <v>83</v>
       </c>
@@ -3629,7 +3639,7 @@
         <v>161</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29"/>
@@ -3640,7 +3650,7 @@
       <c r="H69" s="29"/>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30">
       <c r="A70" s="29" t="s">
         <v>84</v>
       </c>
@@ -3648,7 +3658,7 @@
         <v>161</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29"/>
@@ -3659,7 +3669,7 @@
       <c r="H70" s="29"/>
       <c r="I70" s="31"/>
     </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30">
       <c r="A71" s="29" t="s">
         <v>85</v>
       </c>
@@ -3667,7 +3677,7 @@
         <v>161</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29"/>
@@ -3678,7 +3688,7 @@
       <c r="H71" s="29"/>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="29" t="s">
         <v>86</v>
       </c>
@@ -3686,7 +3696,7 @@
         <v>161</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29"/>
@@ -3697,7 +3707,7 @@
       <c r="H72" s="29"/>
       <c r="I72" s="31"/>
     </row>
-    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="30">
       <c r="A73" s="29" t="s">
         <v>87</v>
       </c>
@@ -3705,7 +3715,7 @@
         <v>161</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -3716,7 +3726,7 @@
       <c r="H73" s="29"/>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="45">
       <c r="A74" s="29" t="s">
         <v>88</v>
       </c>
@@ -3724,7 +3734,7 @@
         <v>161</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29"/>
@@ -3735,7 +3745,7 @@
       <c r="H74" s="29"/>
       <c r="I74" s="31"/>
     </row>
-    <row r="75" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="60">
       <c r="A75" s="29" t="s">
         <v>89</v>
       </c>
@@ -3743,7 +3753,7 @@
         <v>161</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="29"/>
@@ -3754,7 +3764,7 @@
       <c r="H75" s="29"/>
       <c r="I75" s="31"/>
     </row>
-    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="45">
       <c r="A76" s="29" t="s">
         <v>90</v>
       </c>
@@ -3762,7 +3772,7 @@
         <v>161</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29"/>
@@ -3773,7 +3783,7 @@
       <c r="H76" s="29"/>
       <c r="I76" s="31"/>
     </row>
-    <row r="77" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="45">
       <c r="A77" s="29" t="s">
         <v>91</v>
       </c>
@@ -3781,7 +3791,7 @@
         <v>161</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D77" s="29"/>
       <c r="E77" s="29"/>
@@ -3792,7 +3802,7 @@
       <c r="H77" s="29"/>
       <c r="I77" s="31"/>
     </row>
-    <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="60">
       <c r="A78" s="29" t="s">
         <v>92</v>
       </c>
@@ -3800,7 +3810,7 @@
         <v>161</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D78" s="29"/>
       <c r="E78" s="29"/>
@@ -3811,7 +3821,7 @@
       <c r="H78" s="29"/>
       <c r="I78" s="31"/>
     </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="60">
       <c r="A79" s="29" t="s">
         <v>93</v>
       </c>
@@ -3819,7 +3829,7 @@
         <v>161</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D79" s="29"/>
       <c r="E79" s="29"/>
@@ -3830,7 +3840,7 @@
       <c r="H79" s="29"/>
       <c r="I79" s="31"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="29" t="s">
         <v>94</v>
       </c>
@@ -3838,7 +3848,7 @@
         <v>161</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29"/>
@@ -3849,7 +3859,7 @@
       <c r="H80" s="29"/>
       <c r="I80" s="31"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30">
       <c r="A81" s="29" t="s">
         <v>95</v>
       </c>
@@ -3857,7 +3867,7 @@
         <v>161</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D81" s="29"/>
       <c r="E81" s="29"/>
@@ -3868,7 +3878,7 @@
       <c r="H81" s="29"/>
       <c r="I81" s="31"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="30">
       <c r="A82" s="29" t="s">
         <v>96</v>
       </c>
@@ -3876,7 +3886,7 @@
         <v>161</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D82" s="29"/>
       <c r="E82" s="29"/>
@@ -3887,7 +3897,7 @@
       <c r="H82" s="29"/>
       <c r="I82" s="31"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30">
       <c r="A83" s="29" t="s">
         <v>97</v>
       </c>
@@ -3895,7 +3905,7 @@
         <v>161</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="29"/>
@@ -3906,7 +3916,7 @@
       <c r="H83" s="29"/>
       <c r="I83" s="31"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30">
       <c r="A84" s="29" t="s">
         <v>98</v>
       </c>
@@ -3914,7 +3924,7 @@
         <v>161</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D84" s="29"/>
       <c r="E84" s="29"/>
@@ -3925,7 +3935,7 @@
       <c r="H84" s="29"/>
       <c r="I84" s="31"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30">
       <c r="A85" s="29" t="s">
         <v>99</v>
       </c>
@@ -3933,7 +3943,7 @@
         <v>161</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D85" s="29"/>
       <c r="E85" s="29"/>
@@ -3944,7 +3954,7 @@
       <c r="H85" s="29"/>
       <c r="I85" s="31"/>
     </row>
-    <row r="86" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="75">
       <c r="A86" s="29" t="s">
         <v>100</v>
       </c>
@@ -3952,7 +3962,7 @@
         <v>161</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="29"/>
@@ -3963,7 +3973,7 @@
       <c r="H86" s="29"/>
       <c r="I86" s="31"/>
     </row>
-    <row r="87" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="60">
       <c r="A87" s="29" t="s">
         <v>101</v>
       </c>
@@ -3971,7 +3981,7 @@
         <v>161</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29"/>
@@ -3982,7 +3992,7 @@
       <c r="H87" s="29"/>
       <c r="I87" s="31"/>
     </row>
-    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30">
       <c r="A88" s="29" t="s">
         <v>102</v>
       </c>
@@ -3990,7 +4000,7 @@
         <v>161</v>
       </c>
       <c r="C88" s="31" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29"/>
@@ -4001,7 +4011,7 @@
       <c r="H88" s="29"/>
       <c r="I88" s="31"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="30">
       <c r="A89" s="29" t="s">
         <v>103</v>
       </c>
@@ -4009,7 +4019,7 @@
         <v>161</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29"/>
@@ -4020,7 +4030,7 @@
       <c r="H89" s="29"/>
       <c r="I89" s="31"/>
     </row>
-    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="30">
       <c r="A90" s="29" t="s">
         <v>104</v>
       </c>
@@ -4028,7 +4038,7 @@
         <v>161</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29"/>
@@ -4039,7 +4049,7 @@
       <c r="H90" s="29"/>
       <c r="I90" s="31"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9">
       <c r="A91" s="29" t="s">
         <v>105</v>
       </c>
@@ -4047,7 +4057,7 @@
         <v>161</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29"/>
@@ -4058,7 +4068,7 @@
       <c r="H91" s="29"/>
       <c r="I91" s="31"/>
     </row>
-    <row r="92" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="75">
       <c r="A92" s="29" t="s">
         <v>106</v>
       </c>
@@ -4066,7 +4076,7 @@
         <v>161</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29"/>
@@ -4077,7 +4087,7 @@
       <c r="H92" s="29"/>
       <c r="I92" s="31"/>
     </row>
-    <row r="93" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="75">
       <c r="A93" s="29" t="s">
         <v>107</v>
       </c>
@@ -4085,7 +4095,7 @@
         <v>161</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29"/>
@@ -4096,129 +4106,129 @@
       <c r="H93" s="29"/>
       <c r="I93" s="31"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B94" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C94" s="31" t="s">
-        <v>244</v>
+    <row r="94" spans="1:9">
+      <c r="A94" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="B94" s="33">
+        <v>2.4</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>286</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
-      <c r="G94" s="29" t="s">
-        <v>15</v>
+      <c r="G94" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="H94" s="29"/>
       <c r="I94" s="31"/>
     </row>
-    <row r="95" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C95" s="31" t="s">
-        <v>245</v>
+    <row r="95" spans="1:9" ht="30">
+      <c r="A95" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="B95" s="33">
+        <v>2.4</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>287</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="29"/>
       <c r="F95" s="29"/>
-      <c r="G95" s="29" t="s">
+      <c r="G95" s="22" t="s">
         <v>16</v>
       </c>
       <c r="H95" s="29"/>
       <c r="I95" s="31"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B96" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="C96" s="31" t="s">
-        <v>246</v>
+    <row r="96" spans="1:9" ht="30">
+      <c r="A96" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="B96" s="33">
+        <v>2.4</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>299</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="29"/>
       <c r="F96" s="29"/>
-      <c r="G96" s="29" t="s">
-        <v>16</v>
+      <c r="G96" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="H96" s="29"/>
       <c r="I96" s="31"/>
     </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30">
       <c r="A97" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B97" s="30" t="s">
-        <v>163</v>
+        <v>108</v>
+      </c>
+      <c r="B97" s="33">
+        <v>2.5</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29"/>
       <c r="F97" s="29"/>
       <c r="G97" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H97" s="29"/>
       <c r="I97" s="31"/>
     </row>
-    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="45">
       <c r="A98" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="B98" s="30" t="s">
-        <v>163</v>
+        <v>109</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>162</v>
       </c>
       <c r="C98" s="31" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="29"/>
       <c r="F98" s="29"/>
       <c r="G98" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H98" s="29"/>
       <c r="I98" s="31"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9">
       <c r="A99" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="C99" s="31" t="s">
-        <v>249</v>
+        <v>110</v>
+      </c>
+      <c r="B99" s="33">
+        <v>2.6</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>288</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="29"/>
       <c r="F99" s="29"/>
       <c r="G99" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H99" s="29"/>
       <c r="I99" s="31"/>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="30">
       <c r="A100" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B100" s="30" t="s">
-        <v>164</v>
+        <v>111</v>
+      </c>
+      <c r="B100" s="33">
+        <v>2.6</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D100" s="29"/>
       <c r="E100" s="29"/>
@@ -4229,15 +4239,15 @@
       <c r="H100" s="29"/>
       <c r="I100" s="31"/>
     </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="B101" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="C101" s="31" t="s">
-        <v>251</v>
+    <row r="101" spans="1:9" ht="30">
+      <c r="A101" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101" s="33">
+        <v>2.6</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>298</v>
       </c>
       <c r="D101" s="29"/>
       <c r="E101" s="29"/>
@@ -4248,15 +4258,15 @@
       <c r="H101" s="29"/>
       <c r="I101" s="31"/>
     </row>
-    <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9">
       <c r="A102" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B102" s="30" t="s">
-        <v>164</v>
+        <v>113</v>
+      </c>
+      <c r="B102" s="33">
+        <v>2.7</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29"/>
@@ -4267,15 +4277,15 @@
       <c r="H102" s="29"/>
       <c r="I102" s="31"/>
     </row>
-    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="30">
       <c r="A103" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B103" s="30" t="s">
-        <v>164</v>
+        <v>114</v>
+      </c>
+      <c r="B103" s="33">
+        <v>2.7</v>
       </c>
       <c r="C103" s="31" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="29"/>
@@ -4286,34 +4296,34 @@
       <c r="H103" s="29"/>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="30">
       <c r="A104" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B104" s="30" t="s">
-        <v>164</v>
+        <v>115</v>
+      </c>
+      <c r="B104" s="33">
+        <v>2.7</v>
       </c>
       <c r="C104" s="31" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29"/>
       <c r="F104" s="29"/>
       <c r="G104" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H104" s="29"/>
       <c r="I104" s="31"/>
     </row>
-    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="30">
       <c r="A105" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B105" s="30" t="s">
-        <v>164</v>
+        <v>116</v>
+      </c>
+      <c r="B105" s="33">
+        <v>2.7</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29"/>
@@ -4324,34 +4334,34 @@
       <c r="H105" s="29"/>
       <c r="I105" s="31"/>
     </row>
-    <row r="106" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="30">
       <c r="A106" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B106" s="30" t="s">
-        <v>164</v>
+        <v>117</v>
+      </c>
+      <c r="B106" s="33">
+        <v>2.7</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="D106" s="29"/>
       <c r="E106" s="29"/>
       <c r="F106" s="29"/>
       <c r="G106" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H106" s="29"/>
       <c r="I106" s="31"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="105">
       <c r="A107" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B107" s="30" t="s">
-        <v>165</v>
+        <v>118</v>
+      </c>
+      <c r="B107" s="33">
+        <v>2.7</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29"/>
@@ -4362,15 +4372,15 @@
       <c r="H107" s="29"/>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30">
       <c r="A108" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B108" s="30" t="s">
-        <v>165</v>
+        <v>119</v>
+      </c>
+      <c r="B108" s="33">
+        <v>2.7</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29"/>
@@ -4381,15 +4391,15 @@
       <c r="H108" s="29"/>
       <c r="I108" s="31"/>
     </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="45">
       <c r="A109" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B109" s="30" t="s">
-        <v>165</v>
+        <v>120</v>
+      </c>
+      <c r="B109" s="33">
+        <v>2.7</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29"/>
@@ -4400,34 +4410,34 @@
       <c r="H109" s="29"/>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30">
       <c r="A110" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B110" s="30" t="s">
-        <v>166</v>
+        <v>121</v>
+      </c>
+      <c r="B110" s="24" t="s">
+        <v>289</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="29"/>
       <c r="F110" s="29"/>
       <c r="G110" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H110" s="29"/>
       <c r="I110" s="31"/>
     </row>
-    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="30">
       <c r="A111" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B111" s="30" t="s">
-        <v>166</v>
+        <v>122</v>
+      </c>
+      <c r="B111" s="24" t="s">
+        <v>289</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="D111" s="29"/>
       <c r="E111" s="29"/>
@@ -4438,53 +4448,53 @@
       <c r="H111" s="29"/>
       <c r="I111" s="31"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="30">
       <c r="A112" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B112" s="30" t="s">
-        <v>166</v>
+        <v>123</v>
+      </c>
+      <c r="B112" s="24" t="s">
+        <v>289</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29"/>
       <c r="F112" s="29"/>
       <c r="G112" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H112" s="29"/>
       <c r="I112" s="31"/>
     </row>
-    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="30">
       <c r="A113" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="B113" s="30" t="s">
-        <v>167</v>
+        <v>124</v>
+      </c>
+      <c r="B113" s="24" t="s">
+        <v>290</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="29"/>
       <c r="F113" s="29"/>
       <c r="G113" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H113" s="29"/>
       <c r="I113" s="31"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="30">
       <c r="A114" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B114" s="30" t="s">
-        <v>168</v>
+        <v>125</v>
+      </c>
+      <c r="B114" s="24" t="s">
+        <v>290</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29"/>
@@ -4495,34 +4505,34 @@
       <c r="H114" s="29"/>
       <c r="I114" s="31"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="30">
       <c r="A115" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B115" s="30" t="s">
-        <v>168</v>
+        <v>126</v>
+      </c>
+      <c r="B115" s="24" t="s">
+        <v>290</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29"/>
       <c r="F115" s="29"/>
       <c r="G115" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H115" s="29"/>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="30">
       <c r="A116" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B116" s="30" t="s">
-        <v>168</v>
+        <v>127</v>
+      </c>
+      <c r="B116" s="24" t="s">
+        <v>291</v>
       </c>
       <c r="C116" s="31" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29"/>
@@ -4533,34 +4543,34 @@
       <c r="H116" s="29"/>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="30">
       <c r="A117" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B117" s="30" t="s">
-        <v>168</v>
+        <v>128</v>
+      </c>
+      <c r="B117" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="29"/>
       <c r="F117" s="29"/>
       <c r="G117" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H117" s="29"/>
       <c r="I117" s="31"/>
     </row>
-    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="30">
       <c r="A118" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B118" s="30" t="s">
-        <v>168</v>
+        <v>129</v>
+      </c>
+      <c r="B118" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="29"/>
@@ -4571,53 +4581,53 @@
       <c r="H118" s="29"/>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9">
       <c r="A119" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B119" s="30" t="s">
-        <v>168</v>
+        <v>130</v>
+      </c>
+      <c r="B119" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29"/>
       <c r="F119" s="29"/>
       <c r="G119" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H119" s="29"/>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9">
       <c r="A120" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B120" s="30" t="s">
-        <v>168</v>
+        <v>131</v>
+      </c>
+      <c r="B120" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D120" s="29"/>
       <c r="E120" s="29"/>
       <c r="F120" s="29"/>
       <c r="G120" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H120" s="29"/>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="30">
       <c r="A121" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B121" s="30" t="s">
-        <v>168</v>
+        <v>132</v>
+      </c>
+      <c r="B121" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29"/>
@@ -4628,15 +4638,15 @@
       <c r="H121" s="29"/>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9">
       <c r="A122" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="B122" s="30" t="s">
-        <v>168</v>
+        <v>133</v>
+      </c>
+      <c r="B122" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C122" s="31" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29"/>
@@ -4647,15 +4657,15 @@
       <c r="H122" s="29"/>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9">
       <c r="A123" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="B123" s="30" t="s">
-        <v>168</v>
+        <v>134</v>
+      </c>
+      <c r="B123" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C123" s="31" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29"/>
@@ -4666,15 +4676,15 @@
       <c r="H123" s="29"/>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="30">
       <c r="A124" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="B124" s="30" t="s">
-        <v>168</v>
+        <v>135</v>
+      </c>
+      <c r="B124" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29"/>
@@ -4685,15 +4695,15 @@
       <c r="H124" s="29"/>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B125" s="30" t="s">
-        <v>168</v>
+        <v>136</v>
+      </c>
+      <c r="B125" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29"/>
@@ -4704,15 +4714,15 @@
       <c r="H125" s="29"/>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9">
       <c r="A126" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="B126" s="30" t="s">
-        <v>168</v>
+        <v>137</v>
+      </c>
+      <c r="B126" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29"/>
@@ -4723,15 +4733,15 @@
       <c r="H126" s="29"/>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="30">
       <c r="A127" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="B127" s="30" t="s">
-        <v>168</v>
+        <v>138</v>
+      </c>
+      <c r="B127" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29"/>
@@ -4742,15 +4752,15 @@
       <c r="H127" s="29"/>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9">
       <c r="A128" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B128" s="30" t="s">
-        <v>168</v>
+        <v>139</v>
+      </c>
+      <c r="B128" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29"/>
@@ -4761,15 +4771,15 @@
       <c r="H128" s="29"/>
       <c r="I128" s="31"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9">
       <c r="A129" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="B129" s="30" t="s">
-        <v>168</v>
+        <v>140</v>
+      </c>
+      <c r="B129" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C129" s="31" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29"/>
@@ -4780,15 +4790,15 @@
       <c r="H129" s="29"/>
       <c r="I129" s="31"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9">
       <c r="A130" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B130" s="30" t="s">
-        <v>168</v>
+        <v>141</v>
+      </c>
+      <c r="B130" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C130" s="31" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29"/>
@@ -4799,15 +4809,15 @@
       <c r="H130" s="29"/>
       <c r="I130" s="31"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9">
       <c r="A131" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B131" s="30" t="s">
-        <v>168</v>
+        <v>142</v>
+      </c>
+      <c r="B131" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29"/>
@@ -4818,15 +4828,15 @@
       <c r="H131" s="29"/>
       <c r="I131" s="31"/>
     </row>
-    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="30">
       <c r="A132" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B132" s="30" t="s">
-        <v>168</v>
+        <v>143</v>
+      </c>
+      <c r="B132" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="29"/>
@@ -4837,15 +4847,15 @@
       <c r="H132" s="29"/>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9">
       <c r="A133" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="B133" s="30" t="s">
-        <v>168</v>
+        <v>144</v>
+      </c>
+      <c r="B133" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="29"/>
@@ -4856,15 +4866,15 @@
       <c r="H133" s="29"/>
       <c r="I133" s="31"/>
     </row>
-    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="30">
       <c r="A134" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="B134" s="30" t="s">
-        <v>169</v>
+        <v>145</v>
+      </c>
+      <c r="B134" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="29"/>
@@ -4875,34 +4885,34 @@
       <c r="H134" s="29"/>
       <c r="I134" s="31"/>
     </row>
-    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="30">
       <c r="A135" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="B135" s="30" t="s">
-        <v>169</v>
+        <v>146</v>
+      </c>
+      <c r="B135" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29"/>
       <c r="F135" s="29"/>
       <c r="G135" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H135" s="29"/>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="30">
       <c r="A136" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B136" s="30" t="s">
-        <v>169</v>
+        <v>147</v>
+      </c>
+      <c r="B136" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="C136" s="31" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29"/>
@@ -4913,15 +4923,15 @@
       <c r="H136" s="29"/>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="30">
       <c r="A137" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B137" s="30" t="s">
-        <v>170</v>
+        <v>148</v>
+      </c>
+      <c r="B137" s="24" t="s">
+        <v>293</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29"/>
@@ -4932,15 +4942,15 @@
       <c r="H137" s="29"/>
       <c r="I137" s="31"/>
     </row>
-    <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="30">
       <c r="A138" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B138" s="30" t="s">
-        <v>170</v>
+        <v>149</v>
+      </c>
+      <c r="B138" s="24" t="s">
+        <v>293</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29"/>
@@ -4951,15 +4961,15 @@
       <c r="H138" s="29"/>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="135">
       <c r="A139" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B139" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="C139" s="31" t="s">
-        <v>288</v>
+        <v>150</v>
+      </c>
+      <c r="B139" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>297</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29"/>
@@ -4970,34 +4980,34 @@
       <c r="H139" s="29"/>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="30">
       <c r="A140" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B140" s="30" t="s">
-        <v>171</v>
+        <v>151</v>
+      </c>
+      <c r="B140" s="33">
+        <v>2.8</v>
       </c>
       <c r="C140" s="31" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="29"/>
       <c r="F140" s="29"/>
       <c r="G140" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H140" s="29"/>
       <c r="I140" s="31"/>
     </row>
-    <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="30">
       <c r="A141" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="B141" s="30" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="B141" s="33">
+        <v>2.8</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29"/>
@@ -5008,13 +5018,70 @@
       <c r="H141" s="29"/>
       <c r="I141" s="31"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="3"/>
-      <c r="B142" s="10"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="3"/>
-      <c r="B143" s="10"/>
+    <row r="142" spans="1:9" ht="30">
+      <c r="A142" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B142" s="33">
+        <v>2.8</v>
+      </c>
+      <c r="C142" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="D142" s="29"/>
+      <c r="E142" s="29"/>
+      <c r="F142" s="29"/>
+      <c r="G142" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H142" s="29"/>
+      <c r="I142" s="31"/>
+    </row>
+    <row r="143" spans="1:9" ht="45">
+      <c r="A143" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C143" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D143" s="29"/>
+      <c r="E143" s="29"/>
+      <c r="F143" s="29"/>
+      <c r="G143" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H143" s="29"/>
+      <c r="I143" s="31"/>
+    </row>
+    <row r="144" spans="1:9" ht="30">
+      <c r="A144" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B144" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C144" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="D144" s="29"/>
+      <c r="E144" s="29"/>
+      <c r="F144" s="29"/>
+      <c r="G144" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H144" s="29"/>
+      <c r="I144" s="31"/>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="3"/>
+      <c r="B145" s="10"/>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="3"/>
+      <c r="B146" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5032,7 +5099,7 @@
     <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H141 A34:I141">
+  <conditionalFormatting sqref="A20:H144 A34:I144">
     <cfRule type="expression" dxfId="32" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -5043,7 +5110,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H141 A34:I141">
+  <conditionalFormatting sqref="A20:H144 A34:I144">
     <cfRule type="expression" dxfId="29" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -5054,7 +5121,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F141">
+  <conditionalFormatting sqref="F20:F144">
     <cfRule type="expression" dxfId="26" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -5062,7 +5129,7 @@
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I141">
+  <conditionalFormatting sqref="I20:I144">
     <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -5073,7 +5140,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I141">
+  <conditionalFormatting sqref="I20:I144">
     <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -5085,20 +5152,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F141">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F144">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E141">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E144">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G141">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G144">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H141">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H144">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5108,7 +5175,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B143 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B142:B146 B19:B141 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>